<commit_message>
Script to make model from dictionary and corpus.
</commit_message>
<xml_diff>
--- a/docs/開発計画書.xlsx
+++ b/docs/開発計画書.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sata\Work\LE\開発合宿\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sata\Work\LE\開発合宿\twitter_analysis\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138B444E-1395-49D9-AAC4-B1A8CFA83FA8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43626976-8295-454E-A503-414B67B89B21}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="計画書" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="86">
   <si>
     <t>補足</t>
     <rPh sb="0" eb="2">
@@ -485,32 +485,6 @@
     </rPh>
     <rPh sb="12" eb="14">
       <t>カクリツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>学習用コーパス, 初期モデル</t>
-    <rPh sb="0" eb="2">
-      <t>ガクシュウ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ヨウ</t>
-    </rPh>
-    <rPh sb="9" eb="11">
-      <t>ショキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>評価方法, 改良されたモデル</t>
-    <rPh sb="0" eb="2">
-      <t>ヒョウカ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ホウホウ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>カイリョウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -752,6 +726,46 @@
     </rPh>
     <rPh sb="417" eb="418">
       <t>カンガ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>gensim で分類モデルを作り評価する</t>
+    <rPh sb="8" eb="10">
+      <t>ブンルイ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ツク</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ヒョウカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Twitter, MongoDB 周りの治具を作った</t>
+    <rPh sb="17" eb="18">
+      <t>マワ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>ジグ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ツク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>開発が遅れによりリスケジュール</t>
+    <rPh sb="0" eb="2">
+      <t>カイハツ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>オク</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -1578,9 +1592,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1588,21 +1599,384 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1614,9 +1988,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1624,9 +1995,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1638,9 +2006,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1652,12 +2017,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1689,353 +2048,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2429,7 +2443,7 @@
   <dimension ref="B1:AO69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="166" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:U27"/>
+      <selection activeCell="S9" sqref="S9:U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -2446,43 +2460,43 @@
     <row r="2" spans="2:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="2"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="45" t="s">
+      <c r="M2" s="163" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="46"/>
+      <c r="N2" s="164"/>
       <c r="O2" s="1"/>
-      <c r="P2" s="45" t="s">
+      <c r="P2" s="163" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="46"/>
+      <c r="Q2" s="164"/>
       <c r="R2" s="4"/>
-      <c r="S2" s="45" t="s">
+      <c r="S2" s="163" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="46"/>
+      <c r="T2" s="164"/>
     </row>
     <row r="3" spans="2:21" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="122" t="s">
+      <c r="B3" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-      <c r="G3" s="122"/>
-      <c r="H3" s="122"/>
-      <c r="I3" s="122"/>
-      <c r="J3" s="122"/>
-      <c r="K3" s="122"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="123"/>
-      <c r="N3" s="124"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="72"/>
       <c r="O3" s="1"/>
-      <c r="P3" s="123"/>
-      <c r="Q3" s="124"/>
+      <c r="P3" s="71"/>
+      <c r="Q3" s="72"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="123"/>
-      <c r="T3" s="124"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="72"/>
     </row>
     <row r="4" spans="2:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="5"/>
@@ -2496,14 +2510,14 @@
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="125"/>
-      <c r="N4" s="126"/>
+      <c r="M4" s="73"/>
+      <c r="N4" s="74"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="125"/>
-      <c r="Q4" s="126"/>
+      <c r="P4" s="73"/>
+      <c r="Q4" s="74"/>
       <c r="R4" s="4"/>
-      <c r="S4" s="125"/>
-      <c r="T4" s="126"/>
+      <c r="S4" s="73"/>
+      <c r="T4" s="74"/>
     </row>
     <row r="5" spans="2:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="5"/>
@@ -2517,22 +2531,22 @@
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="127"/>
-      <c r="N5" s="128"/>
+      <c r="M5" s="75"/>
+      <c r="N5" s="76"/>
       <c r="O5" s="1"/>
-      <c r="P5" s="127"/>
-      <c r="Q5" s="128"/>
+      <c r="P5" s="75"/>
+      <c r="Q5" s="76"/>
       <c r="R5" s="4"/>
-      <c r="S5" s="127"/>
-      <c r="T5" s="128"/>
+      <c r="S5" s="75"/>
+      <c r="T5" s="76"/>
     </row>
     <row r="6" spans="2:21" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="138" t="s">
+      <c r="B6" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="138"/>
-      <c r="D6" s="138"/>
-      <c r="E6" s="138"/>
+      <c r="C6" s="89"/>
+      <c r="D6" s="89"/>
+      <c r="E6" s="89"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="P6" s="1"/>
@@ -2545,114 +2559,122 @@
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="96"/>
-      <c r="M7" s="96"/>
-      <c r="N7" s="97"/>
-      <c r="O7" s="98"/>
-      <c r="P7" s="134" t="s">
+      <c r="D7" s="109"/>
+      <c r="E7" s="109"/>
+      <c r="F7" s="109"/>
+      <c r="G7" s="109"/>
+      <c r="H7" s="109"/>
+      <c r="I7" s="109"/>
+      <c r="J7" s="109"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="110"/>
+      <c r="M7" s="110"/>
+      <c r="N7" s="111"/>
+      <c r="O7" s="112"/>
+      <c r="P7" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="Q7" s="135"/>
-      <c r="R7" s="136"/>
-      <c r="S7" s="134" t="s">
+      <c r="Q7" s="84"/>
+      <c r="R7" s="85"/>
+      <c r="S7" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="T7" s="135"/>
-      <c r="U7" s="140"/>
+      <c r="T7" s="84"/>
+      <c r="U7" s="92"/>
     </row>
     <row r="8" spans="2:21" s="27" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="44" t="s">
+      <c r="C8" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="132"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
-      <c r="H8" s="132"/>
-      <c r="I8" s="132"/>
-      <c r="J8" s="132"/>
-      <c r="K8" s="132"/>
-      <c r="L8" s="132"/>
-      <c r="M8" s="132"/>
-      <c r="N8" s="132"/>
-      <c r="O8" s="133"/>
-      <c r="P8" s="137">
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="82"/>
+      <c r="P8" s="86">
         <v>43592</v>
       </c>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="36"/>
-      <c r="S8" s="139" t="s">
+      <c r="Q8" s="87"/>
+      <c r="R8" s="88"/>
+      <c r="S8" s="90" t="s">
         <v>65</v>
       </c>
-      <c r="T8" s="33"/>
-      <c r="U8" s="34"/>
+      <c r="T8" s="87"/>
+      <c r="U8" s="91"/>
     </row>
     <row r="9" spans="2:21" s="27" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="28"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="66"/>
-      <c r="P9" s="91"/>
-      <c r="Q9" s="92"/>
-      <c r="R9" s="93"/>
-      <c r="S9" s="91"/>
-      <c r="T9" s="92"/>
-      <c r="U9" s="141"/>
+      <c r="B9" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="113" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="114"/>
+      <c r="J9" s="114"/>
+      <c r="K9" s="114"/>
+      <c r="L9" s="114"/>
+      <c r="M9" s="114"/>
+      <c r="N9" s="114"/>
+      <c r="O9" s="115"/>
+      <c r="P9" s="180">
+        <v>43613</v>
+      </c>
+      <c r="Q9" s="96"/>
+      <c r="R9" s="107"/>
+      <c r="S9" s="95" t="s">
+        <v>65</v>
+      </c>
+      <c r="T9" s="96"/>
+      <c r="U9" s="97"/>
     </row>
     <row r="10" spans="2:21" ht="8.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="2:21" s="27" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="68"/>
-      <c r="D11" s="68"/>
-      <c r="E11" s="89" t="s">
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="93" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="90"/>
-      <c r="G11" s="90"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="90"/>
-      <c r="J11" s="90"/>
-      <c r="K11" s="90"/>
-      <c r="L11" s="90"/>
-      <c r="M11" s="129" t="s">
+      <c r="F11" s="94"/>
+      <c r="G11" s="94"/>
+      <c r="H11" s="94"/>
+      <c r="I11" s="94"/>
+      <c r="J11" s="94"/>
+      <c r="K11" s="94"/>
+      <c r="L11" s="94"/>
+      <c r="M11" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="130"/>
-      <c r="O11" s="131"/>
-      <c r="P11" s="89" t="s">
+      <c r="N11" s="78"/>
+      <c r="O11" s="79"/>
+      <c r="P11" s="93" t="s">
         <v>58</v>
       </c>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="90"/>
-      <c r="S11" s="90"/>
-      <c r="T11" s="90"/>
-      <c r="U11" s="69"/>
+      <c r="Q11" s="94"/>
+      <c r="R11" s="94"/>
+      <c r="S11" s="94"/>
+      <c r="T11" s="94"/>
+      <c r="U11" s="62"/>
     </row>
     <row r="12" spans="2:21" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B12" s="8" t="s">
@@ -2679,364 +2701,364 @@
       <c r="U12" s="10"/>
     </row>
     <row r="13" spans="2:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="80" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="81"/>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="81"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="81"/>
-      <c r="P13" s="81"/>
-      <c r="Q13" s="81"/>
-      <c r="R13" s="81"/>
-      <c r="S13" s="81"/>
-      <c r="T13" s="81"/>
-      <c r="U13" s="82"/>
+      <c r="B13" s="98" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="99"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="99"/>
+      <c r="H13" s="99"/>
+      <c r="I13" s="99"/>
+      <c r="J13" s="99"/>
+      <c r="K13" s="99"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="99"/>
+      <c r="N13" s="99"/>
+      <c r="O13" s="99"/>
+      <c r="P13" s="99"/>
+      <c r="Q13" s="99"/>
+      <c r="R13" s="99"/>
+      <c r="S13" s="99"/>
+      <c r="T13" s="99"/>
+      <c r="U13" s="100"/>
     </row>
     <row r="14" spans="2:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="83"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="84"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="84"/>
-      <c r="L14" s="84"/>
-      <c r="M14" s="84"/>
-      <c r="N14" s="84"/>
-      <c r="O14" s="84"/>
-      <c r="P14" s="84"/>
-      <c r="Q14" s="84"/>
-      <c r="R14" s="84"/>
-      <c r="S14" s="84"/>
-      <c r="T14" s="84"/>
-      <c r="U14" s="85"/>
+      <c r="B14" s="101"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="102"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="102"/>
+      <c r="O14" s="102"/>
+      <c r="P14" s="102"/>
+      <c r="Q14" s="102"/>
+      <c r="R14" s="102"/>
+      <c r="S14" s="102"/>
+      <c r="T14" s="102"/>
+      <c r="U14" s="103"/>
     </row>
     <row r="15" spans="2:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15" s="83"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="84"/>
-      <c r="N15" s="84"/>
-      <c r="O15" s="84"/>
-      <c r="P15" s="84"/>
-      <c r="Q15" s="84"/>
-      <c r="R15" s="84"/>
-      <c r="S15" s="84"/>
-      <c r="T15" s="84"/>
-      <c r="U15" s="85"/>
+      <c r="B15" s="101"/>
+      <c r="C15" s="102"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="102"/>
+      <c r="G15" s="102"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="102"/>
+      <c r="J15" s="102"/>
+      <c r="K15" s="102"/>
+      <c r="L15" s="102"/>
+      <c r="M15" s="102"/>
+      <c r="N15" s="102"/>
+      <c r="O15" s="102"/>
+      <c r="P15" s="102"/>
+      <c r="Q15" s="102"/>
+      <c r="R15" s="102"/>
+      <c r="S15" s="102"/>
+      <c r="T15" s="102"/>
+      <c r="U15" s="103"/>
     </row>
     <row r="16" spans="2:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B16" s="83"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="84"/>
-      <c r="L16" s="84"/>
-      <c r="M16" s="84"/>
-      <c r="N16" s="84"/>
-      <c r="O16" s="84"/>
-      <c r="P16" s="84"/>
-      <c r="Q16" s="84"/>
-      <c r="R16" s="84"/>
-      <c r="S16" s="84"/>
-      <c r="T16" s="84"/>
-      <c r="U16" s="85"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="102"/>
+      <c r="H16" s="102"/>
+      <c r="I16" s="102"/>
+      <c r="J16" s="102"/>
+      <c r="K16" s="102"/>
+      <c r="L16" s="102"/>
+      <c r="M16" s="102"/>
+      <c r="N16" s="102"/>
+      <c r="O16" s="102"/>
+      <c r="P16" s="102"/>
+      <c r="Q16" s="102"/>
+      <c r="R16" s="102"/>
+      <c r="S16" s="102"/>
+      <c r="T16" s="102"/>
+      <c r="U16" s="103"/>
     </row>
     <row r="17" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="83"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="84"/>
-      <c r="I17" s="84"/>
-      <c r="J17" s="84"/>
-      <c r="K17" s="84"/>
-      <c r="L17" s="84"/>
-      <c r="M17" s="84"/>
-      <c r="N17" s="84"/>
-      <c r="O17" s="84"/>
-      <c r="P17" s="84"/>
-      <c r="Q17" s="84"/>
-      <c r="R17" s="84"/>
-      <c r="S17" s="84"/>
-      <c r="T17" s="84"/>
-      <c r="U17" s="85"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="102"/>
+      <c r="D17" s="102"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="102"/>
+      <c r="H17" s="102"/>
+      <c r="I17" s="102"/>
+      <c r="J17" s="102"/>
+      <c r="K17" s="102"/>
+      <c r="L17" s="102"/>
+      <c r="M17" s="102"/>
+      <c r="N17" s="102"/>
+      <c r="O17" s="102"/>
+      <c r="P17" s="102"/>
+      <c r="Q17" s="102"/>
+      <c r="R17" s="102"/>
+      <c r="S17" s="102"/>
+      <c r="T17" s="102"/>
+      <c r="U17" s="103"/>
     </row>
     <row r="18" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="83"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
-      <c r="K18" s="84"/>
-      <c r="L18" s="84"/>
-      <c r="M18" s="84"/>
-      <c r="N18" s="84"/>
-      <c r="O18" s="84"/>
-      <c r="P18" s="84"/>
-      <c r="Q18" s="84"/>
-      <c r="R18" s="84"/>
-      <c r="S18" s="84"/>
-      <c r="T18" s="84"/>
-      <c r="U18" s="85"/>
+      <c r="B18" s="101"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="102"/>
+      <c r="H18" s="102"/>
+      <c r="I18" s="102"/>
+      <c r="J18" s="102"/>
+      <c r="K18" s="102"/>
+      <c r="L18" s="102"/>
+      <c r="M18" s="102"/>
+      <c r="N18" s="102"/>
+      <c r="O18" s="102"/>
+      <c r="P18" s="102"/>
+      <c r="Q18" s="102"/>
+      <c r="R18" s="102"/>
+      <c r="S18" s="102"/>
+      <c r="T18" s="102"/>
+      <c r="U18" s="103"/>
     </row>
     <row r="19" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B19" s="83"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
-      <c r="L19" s="84"/>
-      <c r="M19" s="84"/>
-      <c r="N19" s="84"/>
-      <c r="O19" s="84"/>
-      <c r="P19" s="84"/>
-      <c r="Q19" s="84"/>
-      <c r="R19" s="84"/>
-      <c r="S19" s="84"/>
-      <c r="T19" s="84"/>
-      <c r="U19" s="85"/>
+      <c r="B19" s="101"/>
+      <c r="C19" s="102"/>
+      <c r="D19" s="102"/>
+      <c r="E19" s="102"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="102"/>
+      <c r="H19" s="102"/>
+      <c r="I19" s="102"/>
+      <c r="J19" s="102"/>
+      <c r="K19" s="102"/>
+      <c r="L19" s="102"/>
+      <c r="M19" s="102"/>
+      <c r="N19" s="102"/>
+      <c r="O19" s="102"/>
+      <c r="P19" s="102"/>
+      <c r="Q19" s="102"/>
+      <c r="R19" s="102"/>
+      <c r="S19" s="102"/>
+      <c r="T19" s="102"/>
+      <c r="U19" s="103"/>
     </row>
     <row r="20" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B20" s="83"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="84"/>
-      <c r="F20" s="84"/>
-      <c r="G20" s="84"/>
-      <c r="H20" s="84"/>
-      <c r="I20" s="84"/>
-      <c r="J20" s="84"/>
-      <c r="K20" s="84"/>
-      <c r="L20" s="84"/>
-      <c r="M20" s="84"/>
-      <c r="N20" s="84"/>
-      <c r="O20" s="84"/>
-      <c r="P20" s="84"/>
-      <c r="Q20" s="84"/>
-      <c r="R20" s="84"/>
-      <c r="S20" s="84"/>
-      <c r="T20" s="84"/>
-      <c r="U20" s="85"/>
+      <c r="B20" s="101"/>
+      <c r="C20" s="102"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="102"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="102"/>
+      <c r="J20" s="102"/>
+      <c r="K20" s="102"/>
+      <c r="L20" s="102"/>
+      <c r="M20" s="102"/>
+      <c r="N20" s="102"/>
+      <c r="O20" s="102"/>
+      <c r="P20" s="102"/>
+      <c r="Q20" s="102"/>
+      <c r="R20" s="102"/>
+      <c r="S20" s="102"/>
+      <c r="T20" s="102"/>
+      <c r="U20" s="103"/>
     </row>
     <row r="21" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="83"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="84"/>
-      <c r="F21" s="84"/>
-      <c r="G21" s="84"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="84"/>
-      <c r="J21" s="84"/>
-      <c r="K21" s="84"/>
-      <c r="L21" s="84"/>
-      <c r="M21" s="84"/>
-      <c r="N21" s="84"/>
-      <c r="O21" s="84"/>
-      <c r="P21" s="84"/>
-      <c r="Q21" s="84"/>
-      <c r="R21" s="84"/>
-      <c r="S21" s="84"/>
-      <c r="T21" s="84"/>
-      <c r="U21" s="85"/>
+      <c r="B21" s="101"/>
+      <c r="C21" s="102"/>
+      <c r="D21" s="102"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="102"/>
+      <c r="I21" s="102"/>
+      <c r="J21" s="102"/>
+      <c r="K21" s="102"/>
+      <c r="L21" s="102"/>
+      <c r="M21" s="102"/>
+      <c r="N21" s="102"/>
+      <c r="O21" s="102"/>
+      <c r="P21" s="102"/>
+      <c r="Q21" s="102"/>
+      <c r="R21" s="102"/>
+      <c r="S21" s="102"/>
+      <c r="T21" s="102"/>
+      <c r="U21" s="103"/>
     </row>
     <row r="22" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="83"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="84"/>
-      <c r="F22" s="84"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="84"/>
-      <c r="K22" s="84"/>
-      <c r="L22" s="84"/>
-      <c r="M22" s="84"/>
-      <c r="N22" s="84"/>
-      <c r="O22" s="84"/>
-      <c r="P22" s="84"/>
-      <c r="Q22" s="84"/>
-      <c r="R22" s="84"/>
-      <c r="S22" s="84"/>
-      <c r="T22" s="84"/>
-      <c r="U22" s="85"/>
+      <c r="B22" s="101"/>
+      <c r="C22" s="102"/>
+      <c r="D22" s="102"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="102"/>
+      <c r="I22" s="102"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="102"/>
+      <c r="L22" s="102"/>
+      <c r="M22" s="102"/>
+      <c r="N22" s="102"/>
+      <c r="O22" s="102"/>
+      <c r="P22" s="102"/>
+      <c r="Q22" s="102"/>
+      <c r="R22" s="102"/>
+      <c r="S22" s="102"/>
+      <c r="T22" s="102"/>
+      <c r="U22" s="103"/>
     </row>
     <row r="23" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="83"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="84"/>
-      <c r="L23" s="84"/>
-      <c r="M23" s="84"/>
-      <c r="N23" s="84"/>
-      <c r="O23" s="84"/>
-      <c r="P23" s="84"/>
-      <c r="Q23" s="84"/>
-      <c r="R23" s="84"/>
-      <c r="S23" s="84"/>
-      <c r="T23" s="84"/>
-      <c r="U23" s="85"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="102"/>
+      <c r="D23" s="102"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="102"/>
+      <c r="H23" s="102"/>
+      <c r="I23" s="102"/>
+      <c r="J23" s="102"/>
+      <c r="K23" s="102"/>
+      <c r="L23" s="102"/>
+      <c r="M23" s="102"/>
+      <c r="N23" s="102"/>
+      <c r="O23" s="102"/>
+      <c r="P23" s="102"/>
+      <c r="Q23" s="102"/>
+      <c r="R23" s="102"/>
+      <c r="S23" s="102"/>
+      <c r="T23" s="102"/>
+      <c r="U23" s="103"/>
     </row>
     <row r="24" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="83"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="84"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="84"/>
-      <c r="K24" s="84"/>
-      <c r="L24" s="84"/>
-      <c r="M24" s="84"/>
-      <c r="N24" s="84"/>
-      <c r="O24" s="84"/>
-      <c r="P24" s="84"/>
-      <c r="Q24" s="84"/>
-      <c r="R24" s="84"/>
-      <c r="S24" s="84"/>
-      <c r="T24" s="84"/>
-      <c r="U24" s="85"/>
+      <c r="B24" s="101"/>
+      <c r="C24" s="102"/>
+      <c r="D24" s="102"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="102"/>
+      <c r="I24" s="102"/>
+      <c r="J24" s="102"/>
+      <c r="K24" s="102"/>
+      <c r="L24" s="102"/>
+      <c r="M24" s="102"/>
+      <c r="N24" s="102"/>
+      <c r="O24" s="102"/>
+      <c r="P24" s="102"/>
+      <c r="Q24" s="102"/>
+      <c r="R24" s="102"/>
+      <c r="S24" s="102"/>
+      <c r="T24" s="102"/>
+      <c r="U24" s="103"/>
     </row>
     <row r="25" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B25" s="83"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="84"/>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="84"/>
-      <c r="K25" s="84"/>
-      <c r="L25" s="84"/>
-      <c r="M25" s="84"/>
-      <c r="N25" s="84"/>
-      <c r="O25" s="84"/>
-      <c r="P25" s="84"/>
-      <c r="Q25" s="84"/>
-      <c r="R25" s="84"/>
-      <c r="S25" s="84"/>
-      <c r="T25" s="84"/>
-      <c r="U25" s="85"/>
+      <c r="B25" s="101"/>
+      <c r="C25" s="102"/>
+      <c r="D25" s="102"/>
+      <c r="E25" s="102"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="102"/>
+      <c r="I25" s="102"/>
+      <c r="J25" s="102"/>
+      <c r="K25" s="102"/>
+      <c r="L25" s="102"/>
+      <c r="M25" s="102"/>
+      <c r="N25" s="102"/>
+      <c r="O25" s="102"/>
+      <c r="P25" s="102"/>
+      <c r="Q25" s="102"/>
+      <c r="R25" s="102"/>
+      <c r="S25" s="102"/>
+      <c r="T25" s="102"/>
+      <c r="U25" s="103"/>
     </row>
     <row r="26" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B26" s="83"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="84"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="84"/>
-      <c r="J26" s="84"/>
-      <c r="K26" s="84"/>
-      <c r="L26" s="84"/>
-      <c r="M26" s="84"/>
-      <c r="N26" s="84"/>
-      <c r="O26" s="84"/>
-      <c r="P26" s="84"/>
-      <c r="Q26" s="84"/>
-      <c r="R26" s="84"/>
-      <c r="S26" s="84"/>
-      <c r="T26" s="84"/>
-      <c r="U26" s="85"/>
+      <c r="B26" s="101"/>
+      <c r="C26" s="102"/>
+      <c r="D26" s="102"/>
+      <c r="E26" s="102"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="102"/>
+      <c r="I26" s="102"/>
+      <c r="J26" s="102"/>
+      <c r="K26" s="102"/>
+      <c r="L26" s="102"/>
+      <c r="M26" s="102"/>
+      <c r="N26" s="102"/>
+      <c r="O26" s="102"/>
+      <c r="P26" s="102"/>
+      <c r="Q26" s="102"/>
+      <c r="R26" s="102"/>
+      <c r="S26" s="102"/>
+      <c r="T26" s="102"/>
+      <c r="U26" s="103"/>
     </row>
     <row r="27" spans="2:41" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="86"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="87"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="87"/>
-      <c r="N27" s="87"/>
-      <c r="O27" s="87"/>
-      <c r="P27" s="87"/>
-      <c r="Q27" s="87"/>
-      <c r="R27" s="87"/>
-      <c r="S27" s="87"/>
-      <c r="T27" s="87"/>
-      <c r="U27" s="88"/>
+      <c r="B27" s="104"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="105"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="105"/>
+      <c r="G27" s="105"/>
+      <c r="H27" s="105"/>
+      <c r="I27" s="105"/>
+      <c r="J27" s="105"/>
+      <c r="K27" s="105"/>
+      <c r="L27" s="105"/>
+      <c r="M27" s="105"/>
+      <c r="N27" s="105"/>
+      <c r="O27" s="105"/>
+      <c r="P27" s="105"/>
+      <c r="Q27" s="105"/>
+      <c r="R27" s="105"/>
+      <c r="S27" s="105"/>
+      <c r="T27" s="105"/>
+      <c r="U27" s="106"/>
     </row>
     <row r="28" spans="2:41" s="1" customFormat="1" ht="8.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B29" s="145" t="s">
+      <c r="B29" s="142" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="97"/>
-      <c r="D29" s="97"/>
-      <c r="E29" s="97"/>
-      <c r="F29" s="97"/>
-      <c r="G29" s="97"/>
-      <c r="H29" s="97"/>
-      <c r="I29" s="97"/>
-      <c r="J29" s="97"/>
-      <c r="K29" s="97"/>
-      <c r="L29" s="97"/>
-      <c r="M29" s="97"/>
-      <c r="N29" s="97"/>
-      <c r="O29" s="97"/>
-      <c r="P29" s="97"/>
-      <c r="Q29" s="97"/>
-      <c r="R29" s="97"/>
-      <c r="S29" s="97"/>
-      <c r="T29" s="97"/>
-      <c r="U29" s="146"/>
+      <c r="C29" s="111"/>
+      <c r="D29" s="111"/>
+      <c r="E29" s="111"/>
+      <c r="F29" s="111"/>
+      <c r="G29" s="111"/>
+      <c r="H29" s="111"/>
+      <c r="I29" s="111"/>
+      <c r="J29" s="111"/>
+      <c r="K29" s="111"/>
+      <c r="L29" s="111"/>
+      <c r="M29" s="111"/>
+      <c r="N29" s="111"/>
+      <c r="O29" s="111"/>
+      <c r="P29" s="111"/>
+      <c r="Q29" s="111"/>
+      <c r="R29" s="111"/>
+      <c r="S29" s="111"/>
+      <c r="T29" s="111"/>
+      <c r="U29" s="143"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="AA29" s="1"/>
@@ -3056,30 +3078,30 @@
       <c r="AO29" s="1"/>
     </row>
     <row r="30" spans="2:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B30" s="115" t="s">
+      <c r="B30" s="132" t="s">
         <v>26</v>
       </c>
-      <c r="C30" s="116"/>
-      <c r="D30" s="116"/>
-      <c r="E30" s="116"/>
-      <c r="F30" s="116"/>
-      <c r="G30" s="116"/>
-      <c r="H30" s="116"/>
-      <c r="I30" s="116"/>
-      <c r="J30" s="117" t="s">
+      <c r="C30" s="133"/>
+      <c r="D30" s="133"/>
+      <c r="E30" s="133"/>
+      <c r="F30" s="133"/>
+      <c r="G30" s="133"/>
+      <c r="H30" s="133"/>
+      <c r="I30" s="133"/>
+      <c r="J30" s="134" t="s">
         <v>60</v>
       </c>
-      <c r="K30" s="117"/>
-      <c r="L30" s="117"/>
-      <c r="M30" s="117"/>
-      <c r="N30" s="117"/>
-      <c r="O30" s="117"/>
-      <c r="P30" s="117"/>
-      <c r="Q30" s="117"/>
-      <c r="R30" s="117"/>
-      <c r="S30" s="117"/>
-      <c r="T30" s="117"/>
-      <c r="U30" s="118"/>
+      <c r="K30" s="134"/>
+      <c r="L30" s="134"/>
+      <c r="M30" s="134"/>
+      <c r="N30" s="134"/>
+      <c r="O30" s="134"/>
+      <c r="P30" s="134"/>
+      <c r="Q30" s="134"/>
+      <c r="R30" s="134"/>
+      <c r="S30" s="134"/>
+      <c r="T30" s="134"/>
+      <c r="U30" s="135"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="AA30" s="1"/>
@@ -3099,30 +3121,30 @@
       <c r="AO30" s="1"/>
     </row>
     <row r="31" spans="2:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="115" t="s">
+      <c r="B31" s="132" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="116"/>
-      <c r="D31" s="116"/>
-      <c r="E31" s="116"/>
-      <c r="F31" s="116"/>
-      <c r="G31" s="116"/>
-      <c r="H31" s="116"/>
-      <c r="I31" s="116"/>
-      <c r="J31" s="119" t="s">
+      <c r="C31" s="133"/>
+      <c r="D31" s="133"/>
+      <c r="E31" s="133"/>
+      <c r="F31" s="133"/>
+      <c r="G31" s="133"/>
+      <c r="H31" s="133"/>
+      <c r="I31" s="133"/>
+      <c r="J31" s="136" t="s">
         <v>59</v>
       </c>
-      <c r="K31" s="120"/>
-      <c r="L31" s="120"/>
-      <c r="M31" s="120"/>
-      <c r="N31" s="120"/>
-      <c r="O31" s="120"/>
-      <c r="P31" s="120"/>
-      <c r="Q31" s="120"/>
-      <c r="R31" s="120"/>
-      <c r="S31" s="120"/>
-      <c r="T31" s="120"/>
-      <c r="U31" s="121"/>
+      <c r="K31" s="137"/>
+      <c r="L31" s="137"/>
+      <c r="M31" s="137"/>
+      <c r="N31" s="137"/>
+      <c r="O31" s="137"/>
+      <c r="P31" s="137"/>
+      <c r="Q31" s="137"/>
+      <c r="R31" s="137"/>
+      <c r="S31" s="137"/>
+      <c r="T31" s="137"/>
+      <c r="U31" s="138"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="AA31" s="1"/>
@@ -3142,30 +3164,30 @@
       <c r="AO31" s="1"/>
     </row>
     <row r="32" spans="2:41" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="104" t="s">
+      <c r="B32" s="122" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="105"/>
-      <c r="D32" s="105"/>
-      <c r="E32" s="105"/>
-      <c r="F32" s="105"/>
-      <c r="G32" s="105"/>
-      <c r="H32" s="105"/>
-      <c r="I32" s="105"/>
-      <c r="J32" s="53" t="s">
-        <v>82</v>
-      </c>
-      <c r="K32" s="54"/>
-      <c r="L32" s="54"/>
-      <c r="M32" s="54"/>
-      <c r="N32" s="54"/>
-      <c r="O32" s="100"/>
-      <c r="P32" s="53"/>
-      <c r="Q32" s="54"/>
-      <c r="R32" s="54"/>
-      <c r="S32" s="54"/>
-      <c r="T32" s="54"/>
-      <c r="U32" s="55"/>
+      <c r="C32" s="123"/>
+      <c r="D32" s="123"/>
+      <c r="E32" s="123"/>
+      <c r="F32" s="123"/>
+      <c r="G32" s="123"/>
+      <c r="H32" s="123"/>
+      <c r="I32" s="123"/>
+      <c r="J32" s="116" t="s">
+        <v>80</v>
+      </c>
+      <c r="K32" s="117"/>
+      <c r="L32" s="117"/>
+      <c r="M32" s="117"/>
+      <c r="N32" s="117"/>
+      <c r="O32" s="118"/>
+      <c r="P32" s="116"/>
+      <c r="Q32" s="117"/>
+      <c r="R32" s="117"/>
+      <c r="S32" s="117"/>
+      <c r="T32" s="117"/>
+      <c r="U32" s="170"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="AA32" s="1"/>
@@ -3185,34 +3207,34 @@
       <c r="AO32" s="1"/>
     </row>
     <row r="33" spans="2:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="157" t="s">
+      <c r="B33" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="158"/>
-      <c r="D33" s="106" t="s">
+      <c r="C33" s="38"/>
+      <c r="D33" s="124" t="s">
         <v>24</v>
       </c>
-      <c r="E33" s="107"/>
-      <c r="F33" s="107"/>
-      <c r="G33" s="107"/>
-      <c r="H33" s="107"/>
-      <c r="I33" s="108"/>
-      <c r="J33" s="56" t="s">
+      <c r="E33" s="125"/>
+      <c r="F33" s="125"/>
+      <c r="G33" s="125"/>
+      <c r="H33" s="125"/>
+      <c r="I33" s="126"/>
+      <c r="J33" s="171" t="s">
         <v>61</v>
       </c>
-      <c r="K33" s="57"/>
-      <c r="L33" s="57"/>
-      <c r="M33" s="57"/>
-      <c r="N33" s="57"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="142" t="s">
+      <c r="K33" s="172"/>
+      <c r="L33" s="172"/>
+      <c r="M33" s="172"/>
+      <c r="N33" s="172"/>
+      <c r="O33" s="173"/>
+      <c r="P33" s="139" t="s">
         <v>64</v>
       </c>
-      <c r="Q33" s="143"/>
-      <c r="R33" s="143"/>
-      <c r="S33" s="143"/>
-      <c r="T33" s="143"/>
-      <c r="U33" s="144"/>
+      <c r="Q33" s="140"/>
+      <c r="R33" s="140"/>
+      <c r="S33" s="140"/>
+      <c r="T33" s="140"/>
+      <c r="U33" s="141"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="AA33" s="1"/>
@@ -3232,26 +3254,26 @@
       <c r="AO33" s="1"/>
     </row>
     <row r="34" spans="2:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="159"/>
-      <c r="C34" s="158"/>
-      <c r="D34" s="109"/>
-      <c r="E34" s="110"/>
-      <c r="F34" s="110"/>
-      <c r="G34" s="110"/>
-      <c r="H34" s="110"/>
-      <c r="I34" s="111"/>
-      <c r="J34" s="59"/>
-      <c r="K34" s="60"/>
-      <c r="L34" s="60"/>
-      <c r="M34" s="60"/>
-      <c r="N34" s="60"/>
-      <c r="O34" s="61"/>
-      <c r="P34" s="109"/>
-      <c r="Q34" s="155"/>
-      <c r="R34" s="155"/>
-      <c r="S34" s="155"/>
-      <c r="T34" s="155"/>
-      <c r="U34" s="156"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="127"/>
+      <c r="F34" s="127"/>
+      <c r="G34" s="127"/>
+      <c r="H34" s="127"/>
+      <c r="I34" s="128"/>
+      <c r="J34" s="174"/>
+      <c r="K34" s="175"/>
+      <c r="L34" s="175"/>
+      <c r="M34" s="175"/>
+      <c r="N34" s="175"/>
+      <c r="O34" s="176"/>
+      <c r="P34" s="34"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="35"/>
+      <c r="U34" s="36"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
       <c r="AD34" s="1"/>
@@ -3268,26 +3290,26 @@
       <c r="AO34" s="1"/>
     </row>
     <row r="35" spans="2:41" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="159"/>
-      <c r="C35" s="158"/>
-      <c r="D35" s="101"/>
-      <c r="E35" s="102"/>
-      <c r="F35" s="102"/>
-      <c r="G35" s="102"/>
-      <c r="H35" s="102"/>
-      <c r="I35" s="103"/>
-      <c r="J35" s="112"/>
-      <c r="K35" s="113"/>
-      <c r="L35" s="113"/>
-      <c r="M35" s="113"/>
-      <c r="N35" s="113"/>
-      <c r="O35" s="114"/>
-      <c r="P35" s="50"/>
-      <c r="Q35" s="51"/>
-      <c r="R35" s="51"/>
-      <c r="S35" s="51"/>
-      <c r="T35" s="51"/>
-      <c r="U35" s="52"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="38"/>
+      <c r="D35" s="119"/>
+      <c r="E35" s="120"/>
+      <c r="F35" s="120"/>
+      <c r="G35" s="120"/>
+      <c r="H35" s="120"/>
+      <c r="I35" s="121"/>
+      <c r="J35" s="129"/>
+      <c r="K35" s="130"/>
+      <c r="L35" s="130"/>
+      <c r="M35" s="130"/>
+      <c r="N35" s="130"/>
+      <c r="O35" s="131"/>
+      <c r="P35" s="167"/>
+      <c r="Q35" s="168"/>
+      <c r="R35" s="168"/>
+      <c r="S35" s="168"/>
+      <c r="T35" s="168"/>
+      <c r="U35" s="169"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
       <c r="AD35" s="1"/>
@@ -3304,28 +3326,28 @@
       <c r="AO35" s="1"/>
     </row>
     <row r="36" spans="2:41" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="165" t="s">
+      <c r="B36" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="166"/>
-      <c r="D36" s="166"/>
-      <c r="E36" s="166"/>
-      <c r="F36" s="166"/>
-      <c r="G36" s="166"/>
-      <c r="H36" s="166"/>
-      <c r="I36" s="166"/>
-      <c r="J36" s="167"/>
-      <c r="K36" s="168"/>
-      <c r="L36" s="168"/>
-      <c r="M36" s="168"/>
-      <c r="N36" s="168"/>
-      <c r="O36" s="169"/>
-      <c r="P36" s="167"/>
-      <c r="Q36" s="168"/>
-      <c r="R36" s="168"/>
-      <c r="S36" s="168"/>
-      <c r="T36" s="168"/>
-      <c r="U36" s="170"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="51"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="51"/>
+      <c r="N36" s="51"/>
+      <c r="O36" s="52"/>
+      <c r="P36" s="50"/>
+      <c r="Q36" s="51"/>
+      <c r="R36" s="51"/>
+      <c r="S36" s="51"/>
+      <c r="T36" s="51"/>
+      <c r="U36" s="53"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
       <c r="AA36" s="1"/>
@@ -3345,526 +3367,526 @@
       <c r="AO36" s="1"/>
     </row>
     <row r="37" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B37" s="67" t="s">
+      <c r="B37" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="68"/>
-      <c r="D37" s="68"/>
-      <c r="E37" s="68"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="68"/>
-      <c r="H37" s="68"/>
-      <c r="I37" s="68"/>
-      <c r="J37" s="68"/>
-      <c r="K37" s="68"/>
-      <c r="L37" s="68"/>
-      <c r="M37" s="68"/>
-      <c r="N37" s="68"/>
-      <c r="O37" s="68"/>
-      <c r="P37" s="68"/>
-      <c r="Q37" s="68"/>
-      <c r="R37" s="68"/>
-      <c r="S37" s="68"/>
-      <c r="T37" s="68"/>
-      <c r="U37" s="69"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="61"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="61"/>
+      <c r="J37" s="61"/>
+      <c r="K37" s="61"/>
+      <c r="L37" s="61"/>
+      <c r="M37" s="61"/>
+      <c r="N37" s="61"/>
+      <c r="O37" s="61"/>
+      <c r="P37" s="61"/>
+      <c r="Q37" s="61"/>
+      <c r="R37" s="61"/>
+      <c r="S37" s="61"/>
+      <c r="T37" s="61"/>
+      <c r="U37" s="62"/>
     </row>
     <row r="38" spans="2:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B38" s="172" t="s">
+      <c r="B38" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="173"/>
-      <c r="D38" s="173"/>
-      <c r="E38" s="173"/>
-      <c r="F38" s="173"/>
-      <c r="G38" s="173"/>
-      <c r="H38" s="173"/>
-      <c r="I38" s="173"/>
-      <c r="J38" s="173"/>
-      <c r="K38" s="173"/>
-      <c r="L38" s="173"/>
-      <c r="M38" s="173"/>
-      <c r="N38" s="173"/>
-      <c r="O38" s="173"/>
-      <c r="P38" s="173"/>
-      <c r="Q38" s="173"/>
-      <c r="R38" s="173"/>
-      <c r="S38" s="173"/>
-      <c r="T38" s="173"/>
-      <c r="U38" s="174"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="H38" s="64"/>
+      <c r="I38" s="64"/>
+      <c r="J38" s="64"/>
+      <c r="K38" s="64"/>
+      <c r="L38" s="64"/>
+      <c r="M38" s="64"/>
+      <c r="N38" s="64"/>
+      <c r="O38" s="64"/>
+      <c r="P38" s="64"/>
+      <c r="Q38" s="64"/>
+      <c r="R38" s="64"/>
+      <c r="S38" s="64"/>
+      <c r="T38" s="64"/>
+      <c r="U38" s="65"/>
     </row>
     <row r="39" spans="2:41" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="175"/>
-      <c r="C39" s="176"/>
-      <c r="D39" s="176"/>
-      <c r="E39" s="176"/>
-      <c r="F39" s="176"/>
-      <c r="G39" s="176"/>
-      <c r="H39" s="176"/>
-      <c r="I39" s="176"/>
-      <c r="J39" s="176"/>
-      <c r="K39" s="176"/>
-      <c r="L39" s="176"/>
-      <c r="M39" s="176"/>
-      <c r="N39" s="176"/>
-      <c r="O39" s="176"/>
-      <c r="P39" s="176"/>
-      <c r="Q39" s="176"/>
-      <c r="R39" s="176"/>
-      <c r="S39" s="176"/>
-      <c r="T39" s="176"/>
-      <c r="U39" s="177"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="67"/>
+      <c r="F39" s="67"/>
+      <c r="G39" s="67"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="67"/>
+      <c r="J39" s="67"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="67"/>
+      <c r="N39" s="67"/>
+      <c r="O39" s="67"/>
+      <c r="P39" s="67"/>
+      <c r="Q39" s="67"/>
+      <c r="R39" s="67"/>
+      <c r="S39" s="67"/>
+      <c r="T39" s="67"/>
+      <c r="U39" s="68"/>
     </row>
     <row r="40" spans="2:41" ht="8.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
     </row>
     <row r="41" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B41" s="67" t="s">
+      <c r="B41" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="68"/>
-      <c r="D41" s="68"/>
-      <c r="E41" s="68"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="68"/>
-      <c r="H41" s="68"/>
-      <c r="I41" s="68"/>
-      <c r="J41" s="68"/>
-      <c r="K41" s="68"/>
-      <c r="L41" s="68"/>
-      <c r="M41" s="68"/>
-      <c r="N41" s="68"/>
-      <c r="O41" s="68"/>
-      <c r="P41" s="68"/>
-      <c r="Q41" s="68"/>
-      <c r="R41" s="68"/>
-      <c r="S41" s="68"/>
-      <c r="T41" s="68"/>
-      <c r="U41" s="69"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="61"/>
+      <c r="K41" s="61"/>
+      <c r="L41" s="61"/>
+      <c r="M41" s="61"/>
+      <c r="N41" s="61"/>
+      <c r="O41" s="61"/>
+      <c r="P41" s="61"/>
+      <c r="Q41" s="61"/>
+      <c r="R41" s="61"/>
+      <c r="S41" s="61"/>
+      <c r="T41" s="61"/>
+      <c r="U41" s="62"/>
     </row>
     <row r="42" spans="2:41" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B42" s="75" t="s">
+      <c r="B42" s="144" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="76"/>
-      <c r="D42" s="76"/>
-      <c r="E42" s="76"/>
-      <c r="F42" s="76"/>
-      <c r="G42" s="77"/>
-      <c r="H42" s="35" t="s">
+      <c r="C42" s="155"/>
+      <c r="D42" s="155"/>
+      <c r="E42" s="155"/>
+      <c r="F42" s="155"/>
+      <c r="G42" s="156"/>
+      <c r="H42" s="154" t="s">
         <v>34</v>
       </c>
-      <c r="I42" s="76"/>
-      <c r="J42" s="77"/>
-      <c r="K42" s="32" t="s">
+      <c r="I42" s="155"/>
+      <c r="J42" s="156"/>
+      <c r="K42" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="L42" s="160"/>
-      <c r="M42" s="32" t="s">
+      <c r="L42" s="41"/>
+      <c r="M42" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="N42" s="171"/>
-      <c r="O42" s="29" t="s">
+      <c r="N42" s="54"/>
+      <c r="O42" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="P42" s="30"/>
-      <c r="Q42" s="32" t="s">
+      <c r="P42" s="29"/>
+      <c r="Q42" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="R42" s="160"/>
-      <c r="S42" s="160"/>
-      <c r="T42" s="160"/>
-      <c r="U42" s="164"/>
+      <c r="R42" s="41"/>
+      <c r="S42" s="41"/>
+      <c r="T42" s="41"/>
+      <c r="U42" s="47"/>
     </row>
     <row r="43" spans="2:41" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="145" t="s">
         <v>70</v>
       </c>
-      <c r="C43" s="73"/>
-      <c r="D43" s="73"/>
-      <c r="E43" s="73"/>
-      <c r="F43" s="73"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="178" t="s">
+      <c r="C43" s="146"/>
+      <c r="D43" s="146"/>
+      <c r="E43" s="146"/>
+      <c r="F43" s="146"/>
+      <c r="G43" s="147"/>
+      <c r="H43" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="I43" s="56"/>
+      <c r="J43" s="57"/>
+      <c r="K43" s="58" t="s">
+        <v>67</v>
+      </c>
+      <c r="L43" s="59"/>
+      <c r="M43" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="N43" s="59"/>
+      <c r="O43" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="P43" s="59"/>
+      <c r="Q43" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="R43" s="32"/>
+      <c r="S43" s="32"/>
+      <c r="T43" s="32"/>
+      <c r="U43" s="33"/>
+    </row>
+    <row r="44" spans="2:41" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B44" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="I43" s="179"/>
-      <c r="J43" s="180"/>
-      <c r="K43" s="147" t="s">
-        <v>67</v>
-      </c>
-      <c r="L43" s="148"/>
-      <c r="M43" s="147" t="s">
-        <v>68</v>
-      </c>
-      <c r="N43" s="148"/>
-      <c r="O43" s="147" t="s">
-        <v>69</v>
-      </c>
-      <c r="P43" s="148"/>
-      <c r="Q43" s="152" t="s">
+      <c r="C44" s="146"/>
+      <c r="D44" s="146"/>
+      <c r="E44" s="146"/>
+      <c r="F44" s="146"/>
+      <c r="G44" s="147"/>
+      <c r="H44" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="I44" s="56"/>
+      <c r="J44" s="57"/>
+      <c r="K44" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="L44" s="59"/>
+      <c r="M44" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="N44" s="59"/>
+      <c r="O44" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="P44" s="59"/>
+      <c r="Q44" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="R44" s="32"/>
+      <c r="S44" s="32"/>
+      <c r="T44" s="32"/>
+      <c r="U44" s="33"/>
+    </row>
+    <row r="45" spans="2:41" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B45" s="145" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="146"/>
+      <c r="D45" s="146"/>
+      <c r="E45" s="146"/>
+      <c r="F45" s="146"/>
+      <c r="G45" s="147"/>
+      <c r="H45" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="I45" s="56"/>
+      <c r="J45" s="57"/>
+      <c r="K45" s="58" t="s">
         <v>77</v>
       </c>
-      <c r="R43" s="153"/>
-      <c r="S43" s="153"/>
-      <c r="T43" s="153"/>
-      <c r="U43" s="154"/>
-    </row>
-    <row r="44" spans="2:41" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B44" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="73"/>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="73"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="178" t="s">
-        <v>72</v>
-      </c>
-      <c r="I44" s="179"/>
-      <c r="J44" s="180"/>
-      <c r="K44" s="147" t="s">
+      <c r="L45" s="59"/>
+      <c r="M45" s="58" t="s">
+        <v>78</v>
+      </c>
+      <c r="N45" s="59"/>
+      <c r="O45" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="P45" s="59"/>
+      <c r="Q45" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="L44" s="148"/>
-      <c r="M44" s="147" t="s">
-        <v>74</v>
-      </c>
-      <c r="N44" s="148"/>
-      <c r="O44" s="147" t="s">
-        <v>76</v>
-      </c>
-      <c r="P44" s="148"/>
-      <c r="Q44" s="152" t="s">
-        <v>77</v>
-      </c>
-      <c r="R44" s="153"/>
-      <c r="S44" s="153"/>
-      <c r="T44" s="153"/>
-      <c r="U44" s="154"/>
-    </row>
-    <row r="45" spans="2:41" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B45" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="C45" s="73"/>
-      <c r="D45" s="73"/>
-      <c r="E45" s="73"/>
-      <c r="F45" s="73"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="178" t="s">
-        <v>81</v>
-      </c>
-      <c r="I45" s="179"/>
-      <c r="J45" s="180"/>
-      <c r="K45" s="147" t="s">
-        <v>79</v>
-      </c>
-      <c r="L45" s="148"/>
-      <c r="M45" s="147" t="s">
-        <v>80</v>
-      </c>
-      <c r="N45" s="148"/>
-      <c r="O45" s="147" t="s">
-        <v>76</v>
-      </c>
-      <c r="P45" s="148"/>
-      <c r="Q45" s="152" t="s">
-        <v>77</v>
-      </c>
-      <c r="R45" s="153"/>
-      <c r="S45" s="153"/>
-      <c r="T45" s="153"/>
-      <c r="U45" s="154"/>
+      <c r="R45" s="32"/>
+      <c r="S45" s="32"/>
+      <c r="T45" s="32"/>
+      <c r="U45" s="33"/>
     </row>
     <row r="46" spans="2:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B46" s="40"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="73"/>
-      <c r="G46" s="74"/>
-      <c r="H46" s="70"/>
-      <c r="I46" s="71"/>
-      <c r="J46" s="72"/>
-      <c r="K46" s="147" t="s">
+      <c r="B46" s="145"/>
+      <c r="C46" s="146"/>
+      <c r="D46" s="146"/>
+      <c r="E46" s="146"/>
+      <c r="F46" s="146"/>
+      <c r="G46" s="147"/>
+      <c r="H46" s="151"/>
+      <c r="I46" s="152"/>
+      <c r="J46" s="153"/>
+      <c r="K46" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="L46" s="148"/>
-      <c r="M46" s="147" t="s">
+      <c r="L46" s="59"/>
+      <c r="M46" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="N46" s="148"/>
-      <c r="O46" s="147" t="s">
+      <c r="N46" s="59"/>
+      <c r="O46" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="P46" s="148"/>
-      <c r="Q46" s="152"/>
-      <c r="R46" s="153"/>
-      <c r="S46" s="153"/>
-      <c r="T46" s="153"/>
-      <c r="U46" s="154"/>
+      <c r="P46" s="59"/>
+      <c r="Q46" s="31"/>
+      <c r="R46" s="32"/>
+      <c r="S46" s="32"/>
+      <c r="T46" s="32"/>
+      <c r="U46" s="33"/>
     </row>
     <row r="47" spans="2:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B47" s="40"/>
-      <c r="C47" s="73"/>
-      <c r="D47" s="73"/>
-      <c r="E47" s="73"/>
-      <c r="F47" s="73"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="70"/>
-      <c r="I47" s="71"/>
-      <c r="J47" s="72"/>
-      <c r="K47" s="147" t="s">
+      <c r="B47" s="145"/>
+      <c r="C47" s="146"/>
+      <c r="D47" s="146"/>
+      <c r="E47" s="146"/>
+      <c r="F47" s="146"/>
+      <c r="G47" s="147"/>
+      <c r="H47" s="151"/>
+      <c r="I47" s="152"/>
+      <c r="J47" s="153"/>
+      <c r="K47" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="L47" s="148"/>
-      <c r="M47" s="147" t="s">
+      <c r="L47" s="59"/>
+      <c r="M47" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="N47" s="148"/>
-      <c r="O47" s="147" t="s">
+      <c r="N47" s="59"/>
+      <c r="O47" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="P47" s="148"/>
-      <c r="Q47" s="152"/>
-      <c r="R47" s="153"/>
-      <c r="S47" s="153"/>
-      <c r="T47" s="153"/>
-      <c r="U47" s="154"/>
+      <c r="P47" s="59"/>
+      <c r="Q47" s="31"/>
+      <c r="R47" s="32"/>
+      <c r="S47" s="32"/>
+      <c r="T47" s="32"/>
+      <c r="U47" s="33"/>
     </row>
     <row r="48" spans="2:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B48" s="40"/>
-      <c r="C48" s="73"/>
-      <c r="D48" s="73"/>
-      <c r="E48" s="73"/>
-      <c r="F48" s="73"/>
-      <c r="G48" s="74"/>
-      <c r="H48" s="70"/>
-      <c r="I48" s="71"/>
-      <c r="J48" s="72"/>
-      <c r="K48" s="147" t="s">
+      <c r="B48" s="145"/>
+      <c r="C48" s="146"/>
+      <c r="D48" s="146"/>
+      <c r="E48" s="146"/>
+      <c r="F48" s="146"/>
+      <c r="G48" s="147"/>
+      <c r="H48" s="151"/>
+      <c r="I48" s="152"/>
+      <c r="J48" s="153"/>
+      <c r="K48" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="L48" s="148"/>
-      <c r="M48" s="147" t="s">
+      <c r="L48" s="59"/>
+      <c r="M48" s="58" t="s">
         <v>38</v>
       </c>
-      <c r="N48" s="148"/>
-      <c r="O48" s="147" t="s">
+      <c r="N48" s="59"/>
+      <c r="O48" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="P48" s="148"/>
-      <c r="Q48" s="152"/>
-      <c r="R48" s="153"/>
-      <c r="S48" s="153"/>
-      <c r="T48" s="153"/>
-      <c r="U48" s="154"/>
+      <c r="P48" s="59"/>
+      <c r="Q48" s="31"/>
+      <c r="R48" s="32"/>
+      <c r="S48" s="32"/>
+      <c r="T48" s="32"/>
+      <c r="U48" s="33"/>
     </row>
     <row r="49" spans="2:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="65"/>
-      <c r="C49" s="78"/>
-      <c r="D49" s="78"/>
-      <c r="E49" s="78"/>
-      <c r="F49" s="78"/>
-      <c r="G49" s="79"/>
-      <c r="H49" s="62"/>
-      <c r="I49" s="63"/>
-      <c r="J49" s="64"/>
-      <c r="K49" s="149" t="s">
+      <c r="B49" s="148"/>
+      <c r="C49" s="149"/>
+      <c r="D49" s="149"/>
+      <c r="E49" s="149"/>
+      <c r="F49" s="149"/>
+      <c r="G49" s="150"/>
+      <c r="H49" s="177"/>
+      <c r="I49" s="178"/>
+      <c r="J49" s="179"/>
+      <c r="K49" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="L49" s="151"/>
-      <c r="M49" s="149" t="s">
+      <c r="L49" s="69"/>
+      <c r="M49" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="N49" s="150"/>
-      <c r="O49" s="149" t="s">
+      <c r="N49" s="46"/>
+      <c r="O49" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="P49" s="150"/>
-      <c r="Q49" s="161"/>
-      <c r="R49" s="162"/>
-      <c r="S49" s="162"/>
-      <c r="T49" s="162"/>
-      <c r="U49" s="163"/>
+      <c r="P49" s="46"/>
+      <c r="Q49" s="42"/>
+      <c r="R49" s="43"/>
+      <c r="S49" s="43"/>
+      <c r="T49" s="43"/>
+      <c r="U49" s="44"/>
     </row>
     <row r="50" spans="2:21" ht="8.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="31"/>
-      <c r="K50" s="31"/>
-      <c r="L50" s="31"/>
-      <c r="M50" s="31"/>
-      <c r="N50" s="31"/>
-      <c r="O50" s="31"/>
-      <c r="P50" s="31"/>
-      <c r="Q50" s="31"/>
-      <c r="R50" s="31"/>
-      <c r="S50" s="31"/>
-      <c r="T50" s="31"/>
-      <c r="U50" s="31"/>
+      <c r="B50" s="30"/>
+      <c r="C50" s="30"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="30"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="30"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="30"/>
+      <c r="J50" s="30"/>
+      <c r="K50" s="30"/>
+      <c r="L50" s="30"/>
+      <c r="M50" s="30"/>
+      <c r="N50" s="30"/>
+      <c r="O50" s="30"/>
+      <c r="P50" s="30"/>
+      <c r="Q50" s="30"/>
+      <c r="R50" s="30"/>
+      <c r="S50" s="30"/>
+      <c r="T50" s="30"/>
+      <c r="U50" s="30"/>
     </row>
     <row r="51" spans="2:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B51" s="67" t="s">
+      <c r="B51" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="68"/>
-      <c r="D51" s="68"/>
-      <c r="E51" s="68"/>
-      <c r="F51" s="68"/>
-      <c r="G51" s="68"/>
-      <c r="H51" s="68"/>
-      <c r="I51" s="68"/>
-      <c r="J51" s="68"/>
-      <c r="K51" s="68"/>
-      <c r="L51" s="68"/>
-      <c r="M51" s="68"/>
-      <c r="N51" s="68"/>
-      <c r="O51" s="68"/>
-      <c r="P51" s="68"/>
-      <c r="Q51" s="68"/>
-      <c r="R51" s="68"/>
-      <c r="S51" s="68"/>
-      <c r="T51" s="68"/>
-      <c r="U51" s="69"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="61"/>
+      <c r="G51" s="61"/>
+      <c r="H51" s="61"/>
+      <c r="I51" s="61"/>
+      <c r="J51" s="61"/>
+      <c r="K51" s="61"/>
+      <c r="L51" s="61"/>
+      <c r="M51" s="61"/>
+      <c r="N51" s="61"/>
+      <c r="O51" s="61"/>
+      <c r="P51" s="61"/>
+      <c r="Q51" s="61"/>
+      <c r="R51" s="61"/>
+      <c r="S51" s="61"/>
+      <c r="T51" s="61"/>
+      <c r="U51" s="62"/>
     </row>
     <row r="52" spans="2:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B52" s="75" t="s">
+      <c r="B52" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="C52" s="33"/>
-      <c r="D52" s="33"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="36"/>
-      <c r="J52" s="35" t="s">
+      <c r="C52" s="87"/>
+      <c r="D52" s="87"/>
+      <c r="E52" s="87"/>
+      <c r="F52" s="87"/>
+      <c r="G52" s="87"/>
+      <c r="H52" s="87"/>
+      <c r="I52" s="88"/>
+      <c r="J52" s="154" t="s">
         <v>6</v>
       </c>
-      <c r="K52" s="33"/>
-      <c r="L52" s="33"/>
-      <c r="M52" s="36"/>
-      <c r="N52" s="32" t="s">
+      <c r="K52" s="87"/>
+      <c r="L52" s="87"/>
+      <c r="M52" s="88"/>
+      <c r="N52" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="O52" s="33"/>
-      <c r="P52" s="33"/>
-      <c r="Q52" s="33"/>
-      <c r="R52" s="33"/>
-      <c r="S52" s="33"/>
-      <c r="T52" s="33"/>
-      <c r="U52" s="34"/>
+      <c r="O52" s="87"/>
+      <c r="P52" s="87"/>
+      <c r="Q52" s="87"/>
+      <c r="R52" s="87"/>
+      <c r="S52" s="87"/>
+      <c r="T52" s="87"/>
+      <c r="U52" s="91"/>
     </row>
     <row r="53" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="145" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="33"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="33"/>
-      <c r="H53" s="33"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="41" t="s">
+      <c r="C53" s="87"/>
+      <c r="D53" s="87"/>
+      <c r="E53" s="87"/>
+      <c r="F53" s="87"/>
+      <c r="G53" s="87"/>
+      <c r="H53" s="87"/>
+      <c r="I53" s="88"/>
+      <c r="J53" s="160" t="s">
         <v>62</v>
       </c>
-      <c r="K53" s="42"/>
-      <c r="L53" s="42"/>
-      <c r="M53" s="43"/>
-      <c r="N53" s="44" t="s">
+      <c r="K53" s="161"/>
+      <c r="L53" s="161"/>
+      <c r="M53" s="162"/>
+      <c r="N53" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="O53" s="33"/>
-      <c r="P53" s="33"/>
-      <c r="Q53" s="33"/>
-      <c r="R53" s="33"/>
-      <c r="S53" s="33"/>
-      <c r="T53" s="33"/>
-      <c r="U53" s="34"/>
+      <c r="O53" s="87"/>
+      <c r="P53" s="87"/>
+      <c r="Q53" s="87"/>
+      <c r="R53" s="87"/>
+      <c r="S53" s="87"/>
+      <c r="T53" s="87"/>
+      <c r="U53" s="91"/>
     </row>
     <row r="54" spans="2:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B54" s="40" t="s">
+      <c r="B54" s="145" t="s">
         <v>22</v>
       </c>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="33"/>
-      <c r="I54" s="36"/>
-      <c r="J54" s="41"/>
-      <c r="K54" s="42"/>
-      <c r="L54" s="42"/>
-      <c r="M54" s="43"/>
-      <c r="N54" s="44" t="s">
+      <c r="C54" s="87"/>
+      <c r="D54" s="87"/>
+      <c r="E54" s="87"/>
+      <c r="F54" s="87"/>
+      <c r="G54" s="87"/>
+      <c r="H54" s="87"/>
+      <c r="I54" s="88"/>
+      <c r="J54" s="160"/>
+      <c r="K54" s="161"/>
+      <c r="L54" s="161"/>
+      <c r="M54" s="162"/>
+      <c r="N54" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="O54" s="33"/>
-      <c r="P54" s="33"/>
-      <c r="Q54" s="33"/>
-      <c r="R54" s="33"/>
-      <c r="S54" s="33"/>
-      <c r="T54" s="33"/>
-      <c r="U54" s="34"/>
+      <c r="O54" s="87"/>
+      <c r="P54" s="87"/>
+      <c r="Q54" s="87"/>
+      <c r="R54" s="87"/>
+      <c r="S54" s="87"/>
+      <c r="T54" s="87"/>
+      <c r="U54" s="91"/>
     </row>
     <row r="55" spans="2:21" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="65" t="s">
+      <c r="B55" s="148" t="s">
         <v>32</v>
       </c>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
-      <c r="E55" s="48"/>
-      <c r="F55" s="48"/>
-      <c r="G55" s="48"/>
-      <c r="H55" s="48"/>
-      <c r="I55" s="66"/>
-      <c r="J55" s="37"/>
-      <c r="K55" s="38"/>
-      <c r="L55" s="38"/>
-      <c r="M55" s="39"/>
-      <c r="N55" s="47" t="s">
+      <c r="C55" s="114"/>
+      <c r="D55" s="114"/>
+      <c r="E55" s="114"/>
+      <c r="F55" s="114"/>
+      <c r="G55" s="114"/>
+      <c r="H55" s="114"/>
+      <c r="I55" s="115"/>
+      <c r="J55" s="157"/>
+      <c r="K55" s="158"/>
+      <c r="L55" s="158"/>
+      <c r="M55" s="159"/>
+      <c r="N55" s="165" t="s">
         <v>33</v>
       </c>
-      <c r="O55" s="48"/>
-      <c r="P55" s="48"/>
-      <c r="Q55" s="48"/>
-      <c r="R55" s="48"/>
-      <c r="S55" s="48"/>
-      <c r="T55" s="48"/>
-      <c r="U55" s="49"/>
+      <c r="O55" s="114"/>
+      <c r="P55" s="114"/>
+      <c r="Q55" s="114"/>
+      <c r="R55" s="114"/>
+      <c r="S55" s="114"/>
+      <c r="T55" s="114"/>
+      <c r="U55" s="166"/>
     </row>
     <row r="56" spans="2:21" ht="8.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="31"/>
-      <c r="G56" s="31"/>
-      <c r="H56" s="31"/>
-      <c r="I56" s="31"/>
-      <c r="J56" s="31"/>
-      <c r="K56" s="31"/>
-      <c r="L56" s="31"/>
-      <c r="M56" s="31"/>
-      <c r="N56" s="31"/>
-      <c r="O56" s="31"/>
-      <c r="P56" s="31"/>
-      <c r="Q56" s="31"/>
-      <c r="R56" s="31"/>
-      <c r="S56" s="31"/>
-      <c r="T56" s="31"/>
-      <c r="U56" s="31"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="30"/>
+      <c r="H56" s="30"/>
+      <c r="I56" s="30"/>
+      <c r="J56" s="30"/>
+      <c r="K56" s="30"/>
+      <c r="L56" s="30"/>
+      <c r="M56" s="30"/>
+      <c r="N56" s="30"/>
+      <c r="O56" s="30"/>
+      <c r="P56" s="30"/>
+      <c r="Q56" s="30"/>
+      <c r="R56" s="30"/>
+      <c r="S56" s="30"/>
+      <c r="T56" s="30"/>
+      <c r="U56" s="30"/>
     </row>
     <row r="57" spans="2:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="3" t="s">
@@ -4193,6 +4215,88 @@
     <row r="69" spans="2:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="106">
+    <mergeCell ref="N52:U52"/>
+    <mergeCell ref="J52:M52"/>
+    <mergeCell ref="J55:M55"/>
+    <mergeCell ref="B54:I54"/>
+    <mergeCell ref="B53:I53"/>
+    <mergeCell ref="J53:M53"/>
+    <mergeCell ref="N53:U53"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="J54:M54"/>
+    <mergeCell ref="N54:U54"/>
+    <mergeCell ref="N55:U55"/>
+    <mergeCell ref="P35:U35"/>
+    <mergeCell ref="P32:U32"/>
+    <mergeCell ref="J33:O33"/>
+    <mergeCell ref="J34:O34"/>
+    <mergeCell ref="H49:J49"/>
+    <mergeCell ref="B55:I55"/>
+    <mergeCell ref="B41:U41"/>
+    <mergeCell ref="H48:J48"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B51:U51"/>
+    <mergeCell ref="B52:I52"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B49:G49"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="B43:G43"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B45:G45"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B13:U27"/>
+    <mergeCell ref="E11:L11"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="C7:O7"/>
+    <mergeCell ref="C9:O9"/>
+    <mergeCell ref="J32:O32"/>
+    <mergeCell ref="D35:I35"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="D33:I33"/>
+    <mergeCell ref="D34:I34"/>
+    <mergeCell ref="J35:O35"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="J30:U30"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="J31:U31"/>
+    <mergeCell ref="P33:U33"/>
+    <mergeCell ref="B29:U29"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="M3:N5"/>
+    <mergeCell ref="P3:Q5"/>
+    <mergeCell ref="S3:T5"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="C8:O8"/>
+    <mergeCell ref="P7:R7"/>
+    <mergeCell ref="P8:R8"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="S8:U8"/>
+    <mergeCell ref="S7:U7"/>
+    <mergeCell ref="P11:U11"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="O46:P46"/>
+    <mergeCell ref="O47:P47"/>
+    <mergeCell ref="O48:P48"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="M47:N47"/>
     <mergeCell ref="Q48:U48"/>
     <mergeCell ref="P34:U34"/>
     <mergeCell ref="B33:C35"/>
@@ -4217,88 +4321,6 @@
     <mergeCell ref="B37:U37"/>
     <mergeCell ref="B38:U39"/>
     <mergeCell ref="M48:N48"/>
-    <mergeCell ref="M49:N49"/>
-    <mergeCell ref="O43:P43"/>
-    <mergeCell ref="O44:P44"/>
-    <mergeCell ref="O45:P45"/>
-    <mergeCell ref="O46:P46"/>
-    <mergeCell ref="O47:P47"/>
-    <mergeCell ref="O48:P48"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="M3:N5"/>
-    <mergeCell ref="P3:Q5"/>
-    <mergeCell ref="S3:T5"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="C8:O8"/>
-    <mergeCell ref="P7:R7"/>
-    <mergeCell ref="P8:R8"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="S8:U8"/>
-    <mergeCell ref="S7:U7"/>
-    <mergeCell ref="P11:U11"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="B13:U27"/>
-    <mergeCell ref="E11:L11"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="C7:O7"/>
-    <mergeCell ref="C9:O9"/>
-    <mergeCell ref="J32:O32"/>
-    <mergeCell ref="D35:I35"/>
-    <mergeCell ref="B32:I32"/>
-    <mergeCell ref="D33:I33"/>
-    <mergeCell ref="D34:I34"/>
-    <mergeCell ref="J35:O35"/>
-    <mergeCell ref="B30:I30"/>
-    <mergeCell ref="J30:U30"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="J31:U31"/>
-    <mergeCell ref="P33:U33"/>
-    <mergeCell ref="B29:U29"/>
-    <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B49:G49"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="B43:G43"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B45:G45"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="N52:U52"/>
-    <mergeCell ref="J52:M52"/>
-    <mergeCell ref="J55:M55"/>
-    <mergeCell ref="B54:I54"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="J53:M53"/>
-    <mergeCell ref="N53:U53"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="J54:M54"/>
-    <mergeCell ref="N54:U54"/>
-    <mergeCell ref="N55:U55"/>
-    <mergeCell ref="P35:U35"/>
-    <mergeCell ref="P32:U32"/>
-    <mergeCell ref="J33:O33"/>
-    <mergeCell ref="J34:O34"/>
-    <mergeCell ref="H49:J49"/>
-    <mergeCell ref="B55:I55"/>
-    <mergeCell ref="B41:U41"/>
-    <mergeCell ref="H48:J48"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B51:U51"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.67" right="0.25" top="0.47244094488188981" bottom="0.37" header="0.35433070866141736" footer="0.25"/>
@@ -4306,8 +4328,5 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;C&amp;10&amp;P</oddFooter>
   </headerFooter>
-  <ignoredErrors>
-    <ignoredError sqref="B8" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>